<commit_message>
second commit fully completed excel first page
</commit_message>
<xml_diff>
--- a/datadetails.xlsx
+++ b/datadetails.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -421,7 +421,7 @@
         <v>Sponsor</v>
       </c>
       <c r="B2" t="str">
-        <v>Antony1</v>
+        <v>release-mpfp-binary-business-admin</v>
       </c>
       <c r="C2" t="str">
         <v/>
@@ -451,7 +451,7 @@
         <v>Username</v>
       </c>
       <c r="B5" t="str">
-        <v>raj123</v>
+        <v>raj8955</v>
       </c>
     </row>
     <row r="6">
@@ -459,7 +459,7 @@
         <v>Email address</v>
       </c>
       <c r="B6" t="str">
-        <v>antony123@mailinator.com</v>
+        <v>antony12345@mailinator.com</v>
       </c>
     </row>
     <row r="7">
@@ -469,55 +469,87 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Subdomain</v>
+        <v>Date of Birth</v>
       </c>
       <c r="B8" t="str">
-        <v>antony1</v>
+        <v>1995-08-20</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Phone Number</v>
+        <v>Gender</v>
       </c>
       <c r="B9" t="str">
-        <v>7676656554</v>
+        <v xml:space="preserve">	Male</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Password</v>
+        <v>Subdomain</v>
       </c>
       <c r="B10" t="str">
-        <v>As@12345</v>
+        <v>antony15</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Password Confirm</v>
+        <v>Phone Number</v>
       </c>
       <c r="B11" t="str">
-        <v>As@12345</v>
+        <v>76765477</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Terms and Conditions</v>
+        <v>Password</v>
       </c>
       <c r="B12" t="str">
-        <v>click</v>
+        <v>As@12345</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
+        <v>Password Confirm</v>
+      </c>
+      <c r="B13" t="str">
+        <v>As@12345</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Terms and Conditions</v>
+      </c>
+      <c r="B14" t="str">
+        <v>click</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
         <v>addnew-member</v>
       </c>
-      <c r="B13" t="str">
+      <c r="B15" t="str">
+        <v>click</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v xml:space="preserve">Enrollment Package	</v>
+      </c>
+      <c r="B16" t="str">
+        <v>enrollment-package-10</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Proceed</v>
+      </c>
+      <c r="B17" t="str">
         <v>click</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D13"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Registration selenium python using test payment
</commit_message>
<xml_diff>
--- a/datadetails.xlsx
+++ b/datadetails.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -418,98 +418,98 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Sponsor</v>
+        <v>URL</v>
       </c>
       <c r="B2" t="str">
-        <v>release-mpfp-binary-business-admin</v>
-      </c>
-      <c r="C2" t="str">
-        <v/>
-      </c>
-      <c r="D2" t="str">
-        <v/>
+        <v>https://preprod-matrix.epixel.link/en/register/</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>First Name</v>
+        <v>Sponsor</v>
       </c>
       <c r="B3" t="str">
-        <v>antony</v>
+        <v>release-mpfp-matrix-business-admin</v>
+      </c>
+      <c r="C3" t="str">
+        <v/>
+      </c>
+      <c r="D3" t="str">
+        <v/>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Last Name</v>
+        <v>First Name</v>
       </c>
       <c r="B4" t="str">
-        <v>raj</v>
+        <v>antony</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Username</v>
+        <v>Last Name</v>
       </c>
       <c r="B5" t="str">
-        <v>raj8955</v>
+        <v>raj</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Email address</v>
+        <v>Username</v>
       </c>
       <c r="B6" t="str">
-        <v>antony12345@mailinator.com</v>
+        <v>eyuu0231</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v/>
+        <v>Email address</v>
+      </c>
+      <c r="B7" t="str">
+        <v>abhishna6911@mailinator.com</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Date of Birth</v>
-      </c>
-      <c r="B8" t="str">
-        <v>1995-08-20</v>
+        <v/>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Gender</v>
+        <v>Date of Birth</v>
       </c>
       <c r="B9" t="str">
-        <v xml:space="preserve">	Male</v>
+        <v>1995-08-20</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Subdomain</v>
+        <v>Gender</v>
       </c>
       <c r="B10" t="str">
-        <v>antony15</v>
+        <v xml:space="preserve">	Male</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Phone Number</v>
+        <v>Subdomain</v>
       </c>
       <c r="B11" t="str">
-        <v>76765477</v>
+        <v>abhoii8761</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Password</v>
+        <v>Phone Number</v>
       </c>
       <c r="B12" t="str">
-        <v>As@12345</v>
+        <v>43436701</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Password Confirm</v>
+        <v>Password</v>
       </c>
       <c r="B13" t="str">
         <v>As@12345</v>
@@ -517,15 +517,15 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Terms and Conditions</v>
+        <v>Password Confirm</v>
       </c>
       <c r="B14" t="str">
-        <v>click</v>
+        <v>As@12345</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>addnew-member</v>
+        <v>Terms and Conditions</v>
       </c>
       <c r="B15" t="str">
         <v>click</v>
@@ -533,23 +533,31 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v xml:space="preserve">Enrollment Package	</v>
+        <v>addnew-member</v>
       </c>
       <c r="B16" t="str">
-        <v>enrollment-package-10</v>
+        <v>click</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
+        <v xml:space="preserve">Enrollment Package	</v>
+      </c>
+      <c r="B17" t="str">
+        <v>enrollment-package-9</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
         <v>Proceed</v>
       </c>
-      <c r="B17" t="str">
+      <c r="B18" t="str">
         <v>click</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D17"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D18"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
selenium python-test with change sponsor
</commit_message>
<xml_diff>
--- a/datadetails.xlsx
+++ b/datadetails.xlsx
@@ -421,7 +421,7 @@
         <v>URL</v>
       </c>
       <c r="B2" t="str">
-        <v>https://preprod-matrix.epixel.link/en/register/</v>
+        <v>https://ttri.epixel.link/en/register/</v>
       </c>
     </row>
     <row r="3">
@@ -429,7 +429,7 @@
         <v>Sponsor</v>
       </c>
       <c r="B3" t="str">
-        <v>release-mpfp-matrix-business-admin</v>
+        <v>admin</v>
       </c>
       <c r="C3" t="str">
         <v/>
@@ -459,7 +459,7 @@
         <v>Username</v>
       </c>
       <c r="B6" t="str">
-        <v>eyuu0231</v>
+        <v>ey093134</v>
       </c>
     </row>
     <row r="7">
@@ -467,7 +467,7 @@
         <v>Email address</v>
       </c>
       <c r="B7" t="str">
-        <v>abhishna6911@mailinator.com</v>
+        <v>abhish097@mailinator.com</v>
       </c>
     </row>
     <row r="8">
@@ -496,7 +496,7 @@
         <v>Subdomain</v>
       </c>
       <c r="B11" t="str">
-        <v>abhoii8761</v>
+        <v>akloirt677</v>
       </c>
     </row>
     <row r="12">
@@ -504,7 +504,7 @@
         <v>Phone Number</v>
       </c>
       <c r="B12" t="str">
-        <v>43436701</v>
+        <v>4347870145</v>
       </c>
     </row>
     <row r="13">

</xml_diff>

<commit_message>
excel and random data
</commit_message>
<xml_diff>
--- a/datadetails.xlsx
+++ b/datadetails.xlsx
@@ -459,7 +459,7 @@
         <v>Username</v>
       </c>
       <c r="B6" t="str">
-        <v>ey093134</v>
+        <v>test1913</v>
       </c>
     </row>
     <row r="7">
@@ -467,7 +467,7 @@
         <v>Email address</v>
       </c>
       <c r="B7" t="str">
-        <v>abhish097@mailinator.com</v>
+        <v>Test1234@mailinator.com</v>
       </c>
     </row>
     <row r="8">
@@ -496,7 +496,7 @@
         <v>Subdomain</v>
       </c>
       <c r="B11" t="str">
-        <v>akloirt677</v>
+        <v>test1234</v>
       </c>
     </row>
     <row r="12">
@@ -504,7 +504,7 @@
         <v>Phone Number</v>
       </c>
       <c r="B12" t="str">
-        <v>4347870145</v>
+        <v>434575667</v>
       </c>
     </row>
     <row r="13">

</xml_diff>